<commit_message>
instagramAPI update with location filter to US
</commit_message>
<xml_diff>
--- a/10weekspregnant.xlsx
+++ b/10weekspregnant.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H102"/>
+  <dimension ref="A1:H206"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -577,7 +577,6 @@
           <t>Mikayla Hudson</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
         <v>1084</v>
       </c>
@@ -653,7 +652,6 @@
           <t>CUSTOM HAND DRAWN GRAPHICS</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
         <v>175</v>
       </c>
@@ -1129,7 +1127,6 @@
           <t>𝓜𝓮𝓵𝓲𝓼𝓼𝓪 𝓟𝓸𝓶𝓲𝓼𝓱 IVF Journey</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
         <v>13302</v>
       </c>
@@ -1365,7 +1362,6 @@
           <t>𝐁𝐎𝐃𝐘 𝐁𝐎𝐎𝐒𝐓 𝐌𝐚𝐭𝐞𝐫𝐧𝐢𝐭𝐲 𝐒𝐤𝐢𝐧𝐜𝐚𝐫𝐞</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
         <v>11380</v>
       </c>
@@ -1676,7 +1672,6 @@
           <t>jessadarling</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
@@ -1877,7 +1872,6 @@
           <t>Katie Miller</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr"/>
       <c r="E37" t="n">
         <v>41</v>
       </c>
@@ -2033,7 +2027,6 @@
           <t>Cassie English</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr"/>
       <c r="E41" t="n">
         <v>1741</v>
       </c>
@@ -2549,7 +2542,6 @@
           <t>Joanie (she/her)</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr"/>
       <c r="E54" t="n">
         <v>476</v>
       </c>
@@ -2785,7 +2777,6 @@
           <t>Cassie English</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr"/>
       <c r="E60" t="n">
         <v>1741</v>
       </c>
@@ -3141,7 +3132,6 @@
           <t>Sparkle And Sweat 🦄✨</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr"/>
       <c r="E69" t="n">
         <v>6483</v>
       </c>
@@ -3172,7 +3162,6 @@
           <t>mamimaddymargaritaa</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
@@ -3333,7 +3322,6 @@
           <t>Sparkle And Sweat 🦄✨</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr"/>
       <c r="E74" t="n">
         <v>6483</v>
       </c>
@@ -3929,7 +3917,6 @@
           <t>liz👑</t>
         </is>
       </c>
-      <c r="D89" t="inlineStr"/>
       <c r="E89" t="n">
         <v>95</v>
       </c>
@@ -4245,7 +4232,6 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="D97" t="inlineStr"/>
       <c r="E97" t="n">
         <v>6087</v>
       </c>
@@ -4321,7 +4307,6 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="D99" t="inlineStr"/>
       <c r="E99" t="n">
         <v>6087</v>
       </c>
@@ -4456,6 +4441,4082 @@
         </is>
       </c>
       <c r="H102" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Huntington Beach, California</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>shapebynat</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Natalie Eynon</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>natalie@shapebynat.com</t>
+        </is>
+      </c>
+      <c r="E103" t="n">
+        <v>37243</v>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/shapebynat/</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>2021-02-23</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Carlsbad, California</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>fit_family_fire</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Jessica T</t>
+        </is>
+      </c>
+      <c r="E104" t="n">
+        <v>1765</v>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/fit_family_fire/</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>2021-02-23</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Mandalay Beach</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>britt_saulque</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Brittney Saulque</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>brittneysaulque@aol.com</t>
+        </is>
+      </c>
+      <c r="E105" t="n">
+        <v>13380</v>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/britt_saulque/</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>2021-02-22</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Statesboro, Georgia</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>morgan_sparacio</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Morgan Sparacio</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>morgancoslowfitness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E106" t="n">
+        <v>12382</v>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/morgan_sparacio/</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>2021-02-22</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Carlsbad, California</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>fit_family_fire</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Jessica T</t>
+        </is>
+      </c>
+      <c r="E107" t="n">
+        <v>1765</v>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/fit_family_fire/</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>2021-02-21</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Idaho Falls, Idaho</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>alysinreallife</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Alys (Alice)</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E108" t="n">
+        <v>886</v>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/alysinreallife/</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>2021-02-21</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Fort Foster Park</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>sweet.red.roses13</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Allie Sweet</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E109" t="n">
+        <v>409</v>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sweet.red.roses13/</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>2021-02-21</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Pickerington, Ohio</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>theconfidentmamaco</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>The Confident Mama</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>TheConfidentMamaCo@gmail.com</t>
+        </is>
+      </c>
+      <c r="E110" t="n">
+        <v>332</v>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/theconfidentmamaco/</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>2021-02-18</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>McKinney, Texas</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>modernhomesteadmama</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Victoria🌻Modern Homestead Mama</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>victoria@mymomtasticlife.com</t>
+        </is>
+      </c>
+      <c r="E111" t="n">
+        <v>22572</v>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/modernhomesteadmama/</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>2021-02-17</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Camp Pendleton South</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>five_deep_breaths</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Striving Stoic</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E112" t="n">
+        <v>168</v>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/five_deep_breaths/</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>2021-02-16</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Boston, Massachusetts</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>kayla_mehr_</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Prenatal Postnatal Specialist</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>kaylamehr28@gmail.com</t>
+        </is>
+      </c>
+      <c r="E113" t="n">
+        <v>2228</v>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/kayla_mehr_/</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>2021-02-16</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>4D Imaging LLC</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>4d_imaging</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>4d Imaging LLC</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>info@w2yb.com</t>
+        </is>
+      </c>
+      <c r="E114" t="n">
+        <v>479</v>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/4d_imaging/</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>2021-02-15</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Beaverton, Michigan</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>katiemercerj</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Katie Mercer</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>katiemercer@hotmail.com</t>
+        </is>
+      </c>
+      <c r="E115" t="n">
+        <v>820</v>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/katiemercerj/</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>2021-02-15</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Southaven, Mississippi</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>karli_cummings</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>K A R L I 🌟</t>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>10516</v>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/karli_cummings/</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>2021-02-15</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Reveal</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>reveal3d4dultrasound</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Reveal 3D/4D Ultrasound</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Info@revealaz.com</t>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>420</v>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reveal3d4dultrasound/</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>2021-02-14</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Corpus Christi, Texas</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>krisgillentine</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Kristy Gillentine Callaway 😷</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E118" t="n">
+        <v>1350</v>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/krisgillentine/</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>2021-02-13</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Westlake Village, California</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>carlyamber</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>💫𝙲𝚊𝚛𝚕𝚢 𝙰𝚖𝚋𝚎𝚛💫</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>carlyamberfitness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E119" t="n">
+        <v>10924</v>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/carlyamber/</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>2021-02-12</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Los Angeles, California</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>thejacintofamily</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>The Jacinto Family Blog</t>
+        </is>
+      </c>
+      <c r="E120" t="n">
+        <v>381</v>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/thejacintofamily/</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>2021-02-12</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Hillsboro, Oregon</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>stephanie.lynn.carranza</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Stephanie Carranza</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>scarranz98@gmail.com</t>
+        </is>
+      </c>
+      <c r="E121" t="n">
+        <v>1326</v>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/stephanie.lynn.carranza/</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>2021-02-11</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Gold Bar, Washington</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>jennydaisylove</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>L❣ve&amp;Light✷</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E122" t="n">
+        <v>5043</v>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/jennydaisylove/</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>2021-02-09</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Queens, New York</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>mojoy9415</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>♥ MoJoy ♥</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E123" t="n">
+        <v>166</v>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/mojoy9415/</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>2021-02-08</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Westlake Village, California</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>carlyamber</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>💫𝙲𝚊𝚛𝚕𝚢 𝙰𝚖𝚋𝚎𝚛💫</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>carlyamberfitness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E124" t="n">
+        <v>10924</v>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/carlyamber/</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>2021-02-08</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Lake Geneva, Wisconsin</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>ionelaherescu</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Ionela Herescu</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E125" t="n">
+        <v>260</v>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/ionelaherescu/</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>2021-02-08</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Hillsboro, Oregon</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>stephanie.lynn.carranza</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Stephanie Carranza</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>scarranz98@gmail.com</t>
+        </is>
+      </c>
+      <c r="E126" t="n">
+        <v>1326</v>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/stephanie.lynn.carranza/</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>2021-02-06</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Las Vegas, Nevada</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>meg.gassler</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Megan Gassler 🤍✨🌵</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>vegasinspiredmind@outlook.com</t>
+        </is>
+      </c>
+      <c r="E127" t="n">
+        <v>1281</v>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/meg.gassler/</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>2021-02-05</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Collierville, Tennessee</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>alexcummins89</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Alex Cummins</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E128" t="n">
+        <v>848</v>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/alexcummins89/</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>2021-02-05</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Kalamazoo, Michigan</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>aiminghighermama</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>K A T R I N A  F R E E M A N</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>aiminghighermama@gmail.com</t>
+        </is>
+      </c>
+      <c r="E129" t="n">
+        <v>2919</v>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/aiminghighermama/</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>2021-02-05</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Evansville, Indiana</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>maryrutherford__</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Mary Rutherford</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E130" t="n">
+        <v>857</v>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/maryrutherford__/</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Wit My Baby Daddy</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>keeroyalty</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>•   Caramel Delight  🍯🥵 .</t>
+        </is>
+      </c>
+      <c r="E131" t="n">
+        <v>2426</v>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/keeroyalty/</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>2021-02-05</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Meridian, Idaho</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>kwatson_714</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Katie Watson</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E132" t="n">
+        <v>247</v>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/kwatson_714/</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>2021-02-04</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>San Diego, California</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>jazminnfuentes</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Jazmin Fuentes</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>jazminharo@outlook.com</t>
+        </is>
+      </c>
+      <c r="E133" t="n">
+        <v>3189</v>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/jazminnfuentes/</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>2021-02-04</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Laguna Beach, California</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>travellersoul_world</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Traveller couples</t>
+        </is>
+      </c>
+      <c r="E134" t="n">
+        <v>95</v>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/travellersoul_world/</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>2021-02-04</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Nevada Fertility Center</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>mrs.katbb4me</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Kaitie</t>
+        </is>
+      </c>
+      <c r="E135" t="n">
+        <v>15244</v>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/mrs.katbb4me/</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>2021-02-03</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Chicago, Illinois</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>ranch_stressing</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>KT Hawbaker</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E136" t="n">
+        <v>1629</v>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/ranch_stressing/</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>2021-02-03</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Plymouth, Massachusetts</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>je11_amacfit</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>April MacGilvray (Moore)</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Aprilmarie238@gmail.com</t>
+        </is>
+      </c>
+      <c r="E137" t="n">
+        <v>681</v>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/je11_amacfit/</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>2021-02-03</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Peekskill, New York</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>liaa.garciaa</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>C E L I A</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>garciadcelia@gmail.com</t>
+        </is>
+      </c>
+      <c r="E138" t="n">
+        <v>1861</v>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/liaa.garciaa/</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>2021-02-03</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Rogers Park, Chicago</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>ranch_stressing</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>KT Hawbaker</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E139" t="n">
+        <v>1629</v>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/ranch_stressing/</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>2021-02-03</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Northwest Oklahoma City, Oklahoma City, Oklahoma</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>_kelseypeacock_</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>K E L S E Y  P E A C O C K</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>kelspeacock@gmail.com</t>
+        </is>
+      </c>
+      <c r="E140" t="n">
+        <v>3551</v>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/_kelseypeacock_/</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>2021-02-03</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Alyeska Resort - Girdwood, Alaska</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>yogi_monii</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Monica Duff</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>mlduff@hotmail.com</t>
+        </is>
+      </c>
+      <c r="E141" t="n">
+        <v>1606</v>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/yogi_monii/</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>2021-02-03</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Temecula, California</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>alexfaafetai</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Alex Faafetai🌻♋️</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>alexfaafetai@gmail.com</t>
+        </is>
+      </c>
+      <c r="E142" t="n">
+        <v>7398</v>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/alexfaafetai/</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>2021-02-03</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Palos Verdes Estates, California</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>genniiie</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Gennie</t>
+        </is>
+      </c>
+      <c r="E143" t="n">
+        <v>462</v>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/genniiie/</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>2021-02-02</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Las Vegas, Nevada</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>mrs.katbb4me</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Kaitie</t>
+        </is>
+      </c>
+      <c r="E144" t="n">
+        <v>15244</v>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/mrs.katbb4me/</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>2021-02-02</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Pompano Beach, Florida</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>boombangreveal</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Gender Reveal Balls</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Warren@listdata.com</t>
+        </is>
+      </c>
+      <c r="E145" t="n">
+        <v>791</v>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/boombangreveal/</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>2021-02-02</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Corona, California</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>alexfaafetai</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Alex Faafetai🌻♋️</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>alexfaafetai@gmail.com</t>
+        </is>
+      </c>
+      <c r="E146" t="n">
+        <v>7398</v>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/alexfaafetai/</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>2021-02-01</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Acworth, Georgia</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>catherine.r.schulke</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Catherine Schulke</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>catherinehightower91@gmail.com</t>
+        </is>
+      </c>
+      <c r="E147" t="n">
+        <v>2484</v>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/catherine.r.schulke/</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>2021-02-01</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Pompano Beach, Florida</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>boombangreveal</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Gender Reveal Balls</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Warren@listdata.com</t>
+        </is>
+      </c>
+      <c r="E148" t="n">
+        <v>791</v>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/boombangreveal/</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>2021-02-01</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Riverside, California</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>alexfaafetai</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Alex Faafetai🌻♋️</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>alexfaafetai@gmail.com</t>
+        </is>
+      </c>
+      <c r="E149" t="n">
+        <v>7398</v>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/alexfaafetai/</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>2021-01-31</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Pompano Beach, Florida</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>boombangreveal</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Gender Reveal Balls</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Warren@listdata.com</t>
+        </is>
+      </c>
+      <c r="E150" t="n">
+        <v>791</v>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/boombangreveal/</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>2021-01-31</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Salt Lake City, Utah</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>marliespregnancy</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>My Pregnancy Journey</t>
+        </is>
+      </c>
+      <c r="E151" t="n">
+        <v>59</v>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/marliespregnancy/</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>2021-01-31</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Denver, Colorado</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>katebowensongs</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>kate bowen morse</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E152" t="n">
+        <v>1575</v>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/katebowensongs/</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>2021-01-31</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Pompano Beach, Florida</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>boombangreveal</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Gender Reveal Balls</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Warren@listdata.com</t>
+        </is>
+      </c>
+      <c r="E153" t="n">
+        <v>791</v>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/boombangreveal/</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>2021-01-30</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Rogers Park, Chicago</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>ranch_stressing</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>KT Hawbaker</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E154" t="n">
+        <v>1629</v>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/ranch_stressing/</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>2021-01-30</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Cincinnati,Ohio</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>dr_sedulously.fit</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>𝗗𝗿.𝗦𝗵𝗲𝗿𝗶𝗹𝗹𝗲 𝗦𝗮𝗻𝗱𝗲𝗿𝘀, 𝗣𝗵.𝗗.</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>sedulously.fit@gmail.com</t>
+        </is>
+      </c>
+      <c r="E155" t="n">
+        <v>10542</v>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/dr_sedulously.fit/</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>2021-01-29</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Pompano Beach, Florida</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>boombangreveal</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Gender Reveal Balls</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Warren@listdata.com</t>
+        </is>
+      </c>
+      <c r="E156" t="n">
+        <v>791</v>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/boombangreveal/</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>2021-01-29</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Loyola-Leone Beach</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>ranch_stressing</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>KT Hawbaker</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E157" t="n">
+        <v>1629</v>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/ranch_stressing/</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>2021-01-29</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Loyola-Leone Beach</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>ranch_stressing</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>KT Hawbaker</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E158" t="n">
+        <v>1629</v>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/ranch_stressing/</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>2021-01-29</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Pompano Beach, Florida</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>boombangreveal</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Gender Reveal Balls</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Warren@listdata.com</t>
+        </is>
+      </c>
+      <c r="E159" t="n">
+        <v>791</v>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/boombangreveal/</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>2021-01-27</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Thousand Oaks, California</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>carlyamber</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>💫𝙲𝚊𝚛𝚕𝚢 𝙰𝚖𝚋𝚎𝚛💫</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>carlyamberfitness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E160" t="n">
+        <v>10924</v>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/carlyamber/</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>2021-01-27</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Medford, Oregon</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>graphicnature333</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>₲αββψ</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E161" t="n">
+        <v>329</v>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/graphicnature333/</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>2021-01-25</t>
+        </is>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Malibu, California</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>carlyamber</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>💫𝙲𝚊𝚛𝚕𝚢 𝙰𝚖𝚋𝚎𝚛💫</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>carlyamberfitness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E162" t="n">
+        <v>10924</v>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/carlyamber/</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>2021-01-25</t>
+        </is>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Pompano Beach, Florida</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>boombangreveal</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Gender Reveal Balls</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Warren@listdata.com</t>
+        </is>
+      </c>
+      <c r="E163" t="n">
+        <v>791</v>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/boombangreveal/</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>2021-01-24</t>
+        </is>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Baker's Beach</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>healthymamasandbabies</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Healthymamas</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Amberloopearsonrebirth@gmail.com</t>
+        </is>
+      </c>
+      <c r="E164" t="n">
+        <v>1622</v>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/healthymamasandbabies/</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>2021-01-23</t>
+        </is>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Pembroke Pines, Florida</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>sindyarenas</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>Sindy Arenas</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>contact@sindyarenas.com</t>
+        </is>
+      </c>
+      <c r="E165" t="n">
+        <v>57101</v>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sindyarenas/</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>2021-01-22</t>
+        </is>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>Thousand Oaks, California</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>carlyamber</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>💫𝙲𝚊𝚛𝚕𝚢 𝙰𝚖𝚋𝚎𝚛💫</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>carlyamberfitness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E166" t="n">
+        <v>10924</v>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/carlyamber/</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>2021-01-22</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>Thousand Oaks, California</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>carlyamber</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>💫𝙲𝚊𝚛𝚕𝚢 𝙰𝚖𝚋𝚎𝚛💫</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>carlyamberfitness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E167" t="n">
+        <v>10924</v>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/carlyamber/</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>2021-01-20</t>
+        </is>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>Miller Fitness - Skowhegan, Maine</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>morganstaples_</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>✖️Morgan Staples | Fit Mom✖️</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>morganbuker@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E168" t="n">
+        <v>2155</v>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/morganstaples_/</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>2021-01-20</t>
+        </is>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>Pompano Beach, Florida</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>boombangreveal</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Gender Reveal Balls</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>Warren@listdata.com</t>
+        </is>
+      </c>
+      <c r="E169" t="n">
+        <v>791</v>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/boombangreveal/</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>2021-01-20</t>
+        </is>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>Lafayette, Indiana</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>adasgiftdoulaservices</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Nicole Ramsey</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>adasgiftdoulaservices@gmail.com</t>
+        </is>
+      </c>
+      <c r="E170" t="n">
+        <v>995</v>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/adasgiftdoulaservices/</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>2021-01-19</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>Front Street Cafe Philadelphia</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>fitnessgoddesspa</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>Nina</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>smcgloster@gmail.com</t>
+        </is>
+      </c>
+      <c r="E171" t="n">
+        <v>3836</v>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/fitnessgoddesspa/</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>2021-01-18</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>Front Street Cafe Philadelphia</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>veganmuscle.fit</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Vegan Muscle</t>
+        </is>
+      </c>
+      <c r="E172" t="n">
+        <v>972</v>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/veganmuscle.fit/</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>2021-01-18</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>Front Street Cafe Philadelphia</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>fitnessgoddesspa</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>Nina</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>smcgloster@gmail.com</t>
+        </is>
+      </c>
+      <c r="E173" t="n">
+        <v>3836</v>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/fitnessgoddesspa/</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>2021-01-18</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>Front Street Cafe Philadelphia</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>fitnessgoddesspa</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Nina</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>smcgloster@gmail.com</t>
+        </is>
+      </c>
+      <c r="E174" t="n">
+        <v>3836</v>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/fitnessgoddesspa/</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>2021-01-18</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>Olathe, Kansas</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>thankyoujxy21</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>Jayd'n Blacknoll</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>jaydnblacknoll21@gmail.com</t>
+        </is>
+      </c>
+      <c r="E175" t="n">
+        <v>631</v>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/thankyoujxy21/</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>2021-01-18</t>
+        </is>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>Lafayette, Indiana</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>adasgiftdoulaservices</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Nicole Ramsey</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>adasgiftdoulaservices@gmail.com</t>
+        </is>
+      </c>
+      <c r="E176" t="n">
+        <v>995</v>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/adasgiftdoulaservices/</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>2021-01-18</t>
+        </is>
+      </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>Westlake Village, California</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>carlyamber</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>💫𝙲𝚊𝚛𝚕𝚢 𝙰𝚖𝚋𝚎𝚛💫</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>carlyamberfitness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E177" t="n">
+        <v>10924</v>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/carlyamber/</t>
+        </is>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>2021-01-17</t>
+        </is>
+      </c>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>Thousand Oaks, California</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>carlyamber</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>💫𝙲𝚊𝚛𝚕𝚢 𝙰𝚖𝚋𝚎𝚛💫</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>carlyamberfitness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E178" t="n">
+        <v>10924</v>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/carlyamber/</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>2021-01-16</t>
+        </is>
+      </c>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>Whiting, Iowa</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>joannahobbs_</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>JoAnna Hobbs</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>hannerjoanna@gmail.com</t>
+        </is>
+      </c>
+      <c r="E179" t="n">
+        <v>3142</v>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/joannahobbs_/</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>2021-01-15</t>
+        </is>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>Dr.Arjang Naim 'OB/GYN'</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>dr.arjangnaim</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Arjang Naim MD | OBGYN</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>support@drarjangnaim.com</t>
+        </is>
+      </c>
+      <c r="E180" t="n">
+        <v>2042</v>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/dr.arjangnaim/</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>2021-01-15</t>
+        </is>
+      </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>Gold's Gym SoCal</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>vfitalicia</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Alicia Valenzuela</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E181" t="n">
+        <v>419</v>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/vfitalicia/</t>
+        </is>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>2021-01-15</t>
+        </is>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>Plunge Beach Resort</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>rachelpaige1121</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>Rachel Eisendrath</t>
+        </is>
+      </c>
+      <c r="E182" t="n">
+        <v>772</v>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/rachelpaige1121/</t>
+        </is>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>2021-01-15</t>
+        </is>
+      </c>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>Saint Petersburg, Florida</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>pregnancytreasures</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>Pregnancy Treasures &amp; Boutique</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>desk@pregnancytreasures.com</t>
+        </is>
+      </c>
+      <c r="E183" t="n">
+        <v>2463</v>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/pregnancytreasures/</t>
+        </is>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>2021-01-14</t>
+        </is>
+      </c>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>Manatee, Florida</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>emilyahintze</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>Mom Life, Fitness, Food</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E184" t="n">
+        <v>2099</v>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/emilyahintze/</t>
+        </is>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>2021-01-13</t>
+        </is>
+      </c>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>Poquonock Bridge, Connecticut</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>tristaam</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>Trista Maxson</t>
+        </is>
+      </c>
+      <c r="E185" t="n">
+        <v>386</v>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/tristaam/</t>
+        </is>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>2021-01-13</t>
+        </is>
+      </c>
+      <c r="H185" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>Kansas City, Kansas</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>elysenull</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>elysenull</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>meetthenulls@gmail.com</t>
+        </is>
+      </c>
+      <c r="E186" t="n">
+        <v>11569</v>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/elysenull/</t>
+        </is>
+      </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>2021-01-13</t>
+        </is>
+      </c>
+      <c r="H186" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>Delaware County, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>sghi_nola</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>COMEccME 👻</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E187" t="n">
+        <v>791</v>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sghi_nola/</t>
+        </is>
+      </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>2021-01-13</t>
+        </is>
+      </c>
+      <c r="H187" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>Delaware County, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>be_thee_wave</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>Glowden✨GoAt 🌿🦄🌿</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>cecebarnes93@icloud.com</t>
+        </is>
+      </c>
+      <c r="E188" t="n">
+        <v>200</v>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/be_thee_wave/</t>
+        </is>
+      </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>2021-01-13</t>
+        </is>
+      </c>
+      <c r="H188" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>Madison, Mississippi</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>hellofrankieday</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>Frankie Day</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>hellofrankieday@gmail.com</t>
+        </is>
+      </c>
+      <c r="E189" t="n">
+        <v>14247</v>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/hellofrankieday/</t>
+        </is>
+      </c>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>2021-01-12</t>
+        </is>
+      </c>
+      <c r="H189" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Ferndale, Michigan</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>nichole_corbin</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>Nichole.Corbin.fitness</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E190" t="n">
+        <v>927</v>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/nichole_corbin/</t>
+        </is>
+      </c>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>2021-01-12</t>
+        </is>
+      </c>
+      <c r="H190" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>Ventura Beach Califorina</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>carlyamber</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>💫𝙲𝚊𝚛𝚕𝚢 𝙰𝚖𝚋𝚎𝚛💫</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>carlyamberfitness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E191" t="n">
+        <v>10924</v>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/carlyamber/</t>
+        </is>
+      </c>
+      <c r="G191" t="inlineStr">
+        <is>
+          <t>2021-01-11</t>
+        </is>
+      </c>
+      <c r="H191" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>Stevens Point, Wisconsin</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>portagecountyprolife</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>Pro Life Portage County</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E192" t="n">
+        <v>206</v>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/portagecountyprolife/</t>
+        </is>
+      </c>
+      <c r="G192" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="H192" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>Duncan, South Carolina</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>sydney_garrison_</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>Sydney Garrison</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>EssentiallySydney@gmail.com</t>
+        </is>
+      </c>
+      <c r="E193" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sydney_garrison_/</t>
+        </is>
+      </c>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="H193" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>Maple Grove, Minnesota</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>alvaradogina14</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>Gina🔹Rubio🔹</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E194" t="n">
+        <v>297</v>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/alvaradogina14/</t>
+        </is>
+      </c>
+      <c r="G194" t="inlineStr">
+        <is>
+          <t>2021-01-08</t>
+        </is>
+      </c>
+      <c r="H194" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>Guilderland, New York</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>tracey_zusman</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>Tracey Zusman</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>congirl24@gmail.com</t>
+        </is>
+      </c>
+      <c r="E195" t="n">
+        <v>19165</v>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/tracey_zusman/</t>
+        </is>
+      </c>
+      <c r="G195" t="inlineStr">
+        <is>
+          <t>2021-01-07</t>
+        </is>
+      </c>
+      <c r="H195" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>Yountville, California</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>carly.blessing</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>Carly Blessing</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E196" t="n">
+        <v>604</v>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/carly.blessing/</t>
+        </is>
+      </c>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>2021-01-07</t>
+        </is>
+      </c>
+      <c r="H196" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>Planet Fitness</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>sraerbaehcca.fit</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>Sarah Rebecca</t>
+        </is>
+      </c>
+      <c r="E197" t="n">
+        <v>14</v>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sraerbaehcca.fit/</t>
+        </is>
+      </c>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>2021-01-06</t>
+        </is>
+      </c>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>Melton Hill Park</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>mrsmeganhedley</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>🦖Megan Hedley🦕</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>hedleyfamilyblog@gmail.com</t>
+        </is>
+      </c>
+      <c r="E198" t="n">
+        <v>12346</v>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/mrsmeganhedley/</t>
+        </is>
+      </c>
+      <c r="G198" t="inlineStr">
+        <is>
+          <t>2021-01-06</t>
+        </is>
+      </c>
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>See My Baby Ultrasound</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>et.miz</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>Eric &amp; Tracey</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E199" t="n">
+        <v>29</v>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/et.miz/</t>
+        </is>
+      </c>
+      <c r="G199" t="inlineStr">
+        <is>
+          <t>2021-01-06</t>
+        </is>
+      </c>
+      <c r="H199" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>Guilderland, New York</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>tracey_zusman</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>Tracey Zusman</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>congirl24@gmail.com</t>
+        </is>
+      </c>
+      <c r="E200" t="n">
+        <v>19165</v>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/tracey_zusman/</t>
+        </is>
+      </c>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>2021-01-06</t>
+        </is>
+      </c>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>Lumberton, New Jersey</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>julwelde</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>J U L I E  W E L D E</t>
+        </is>
+      </c>
+      <c r="E201" t="n">
+        <v>10625</v>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/julwelde/</t>
+        </is>
+      </c>
+      <c r="G201" t="inlineStr">
+        <is>
+          <t>2021-01-04</t>
+        </is>
+      </c>
+      <c r="H201" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>Thousand Oaks, California</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>carlyamber</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>💫𝙲𝚊𝚛𝚕𝚢 𝙰𝚖𝚋𝚎𝚛💫</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>carlyamberfitness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E202" t="n">
+        <v>10924</v>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/carlyamber/</t>
+        </is>
+      </c>
+      <c r="G202" t="inlineStr">
+        <is>
+          <t>2021-01-04</t>
+        </is>
+      </c>
+      <c r="H202" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>Pigeon Forge, Tennessee</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>fitness_schmidtness</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>Kerri Steelman-Schmidt</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>KerriSteelmanSchmidt@SheFitFriend.com</t>
+        </is>
+      </c>
+      <c r="E203" t="n">
+        <v>10943</v>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/fitness_schmidtness/</t>
+        </is>
+      </c>
+      <c r="G203" t="inlineStr">
+        <is>
+          <t>2021-01-04</t>
+        </is>
+      </c>
+      <c r="H203" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>Guilderland, New York</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>tracey_zusman</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>Tracey Zusman</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>congirl24@gmail.com</t>
+        </is>
+      </c>
+      <c r="E204" t="n">
+        <v>19165</v>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/tracey_zusman/</t>
+        </is>
+      </c>
+      <c r="G204" t="inlineStr">
+        <is>
+          <t>2021-01-04</t>
+        </is>
+      </c>
+      <c r="H204" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>Saratoga Lake - South Shore</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>tracey_zusman</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>Tracey Zusman</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>congirl24@gmail.com</t>
+        </is>
+      </c>
+      <c r="E205" t="n">
+        <v>19165</v>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/tracey_zusman/</t>
+        </is>
+      </c>
+      <c r="G205" t="inlineStr">
+        <is>
+          <t>2021-01-03</t>
+        </is>
+      </c>
+      <c r="H205" t="inlineStr">
+        <is>
+          <t>10weekspregnant</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>South Dakota</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>sodoroshop</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>Sodoro</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr"/>
+      <c r="E206" t="n">
+        <v>312</v>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sodoroshop/</t>
+        </is>
+      </c>
+      <c r="G206" t="inlineStr">
+        <is>
+          <t>2021-01-03</t>
+        </is>
+      </c>
+      <c r="H206" t="inlineStr">
         <is>
           <t>10weekspregnant</t>
         </is>

</xml_diff>